<commit_message>
Before internal revision by Søren and Mark
</commit_message>
<xml_diff>
--- a/Data/easy_trial_seperate_schemes/_e_visit__vo__max_protokol.mITT.data .xlsx
+++ b/Data/easy_trial_seperate_schemes/_e_visit__vo__max_protokol.mITT.data .xlsx
@@ -7778,7 +7778,7 @@
       </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1	Plateu i VO2</t>
         </is>
       </c>
       <c r="T43">
@@ -8128,7 +8128,7 @@
       </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1</t>
         </is>
       </c>
       <c r="T45">
@@ -8303,7 +8303,7 @@
       </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1</t>
         </is>
       </c>
       <c r="T46">
@@ -8828,7 +8828,7 @@
       </c>
       <c r="S49" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1	Plateu i VO2</t>
         </is>
       </c>
       <c r="T49">
@@ -9178,7 +9178,7 @@
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1	Plateu i VO2</t>
         </is>
       </c>
       <c r="T51">
@@ -9883,17 +9883,17 @@
       </c>
       <c r="S55" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1	Plateu i VO2</t>
         </is>
       </c>
       <c r="T55">
         <v>12</v>
       </c>
       <c r="U55">
-        <v>2158.13</v>
+        <v>2171.22</v>
       </c>
       <c r="V55">
-        <v>29.08</v>
+        <v>29.26</v>
       </c>
       <c r="W55">
         <v>165</v>
@@ -10413,17 +10413,17 @@
       </c>
       <c r="S58" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1</t>
         </is>
       </c>
       <c r="T58">
         <v>13</v>
       </c>
       <c r="U58">
-        <v>995.35</v>
+        <v>993.64</v>
       </c>
       <c r="V58">
-        <v>22.78</v>
+        <v>22.74</v>
       </c>
       <c r="W58">
         <v>118</v>
@@ -11120,10 +11120,10 @@
         <v>9</v>
       </c>
       <c r="U62">
-        <v>1709.92</v>
+        <v>1589.56</v>
       </c>
       <c r="V62">
-        <v>33.01</v>
+        <v>30.69</v>
       </c>
       <c r="W62">
         <v>166</v>
@@ -11288,7 +11288,7 @@
       </c>
       <c r="S63" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0	Plateu i VO2</t>
         </is>
       </c>
       <c r="T63">
@@ -11463,7 +11463,7 @@
       </c>
       <c r="S64" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1	Plateu i VO2</t>
         </is>
       </c>
       <c r="T64">
@@ -13063,7 +13063,7 @@
       </c>
       <c r="S73" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1</t>
         </is>
       </c>
       <c r="T73">
@@ -20286,7 +20286,7 @@
       </c>
       <c r="S114" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1	Plateu i VO2</t>
         </is>
       </c>
       <c r="T114">
@@ -20461,7 +20461,7 @@
       </c>
       <c r="S115" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1	Plateu i VO2</t>
         </is>
       </c>
       <c r="T115">
@@ -21176,7 +21176,7 @@
       </c>
       <c r="S119" t="inlineStr">
         <is>
-          <t>Plateu i VO2</t>
+          <t>0	Plateu i VO2</t>
         </is>
       </c>
       <c r="T119">
@@ -21526,7 +21526,7 @@
       </c>
       <c r="S121" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1	Plateu i VO2</t>
         </is>
       </c>
       <c r="T121">
@@ -21706,7 +21706,7 @@
       </c>
       <c r="S122" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0	Plateu i VO2</t>
         </is>
       </c>
       <c r="T122">
@@ -22948,7 +22948,7 @@
       </c>
       <c r="S129" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0	Plateu i VO2</t>
         </is>
       </c>
       <c r="T129">
@@ -24540,7 +24540,7 @@
       </c>
       <c r="S138" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0	1	Plateu i VO2</t>
         </is>
       </c>
       <c r="T138">
@@ -24715,7 +24715,7 @@
       </c>
       <c r="S139" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0	1	Plateu i VO2</t>
         </is>
       </c>
       <c r="T139">
@@ -25770,17 +25770,17 @@
       </c>
       <c r="S145" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1</t>
         </is>
       </c>
       <c r="T145">
         <v>12</v>
       </c>
       <c r="U145">
-        <v>2724.7</v>
+        <v>2455.64</v>
       </c>
       <c r="V145">
-        <v>46.98</v>
+        <v>42.34</v>
       </c>
       <c r="W145">
         <v>181</v>
@@ -27180,7 +27180,7 @@
       </c>
       <c r="S153" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0	1	Plateu i VO2</t>
         </is>
       </c>
       <c r="T153">

</xml_diff>